<commit_message>
MàJ HPLC and UPLC contraints
</commit_message>
<xml_diff>
--- a/contraintesModelio.xlsx
+++ b/contraintesModelio.xlsx
@@ -27,7 +27,7 @@
     <t xml:space="preserve">has unit: Joules</t>
   </si>
   <si>
-    <t xml:space="preserve">nullable</t>
+    <t xml:space="preserve">nullable : NA, LD, LQ</t>
   </si>
   <si>
     <t xml:space="preserve">has unit: mL</t>
@@ -155,12 +155,12 @@
   <dimension ref="A2:A12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -242,7 +242,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -268,7 +268,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.65"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>